<commit_message>
change in mini cart offer code
change in mini cart offer code
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.Checkout.xlsx
+++ b/lib_testcase/com.aislend.Checkout.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2555" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1640" uniqueCount="287">
   <si>
     <t>Action</t>
   </si>
@@ -697,9 +697,6 @@
     <t>"6000"</t>
   </si>
   <si>
-    <t>Text Entered successfully: 6000</t>
-  </si>
-  <si>
     <t>"068202322"</t>
   </si>
   <si>
@@ -718,9 +715,6 @@
     <t>verify time slot</t>
   </si>
   <si>
-    <t>Text Entered successfully: 068202322</t>
-  </si>
-  <si>
     <t>Time Slot should not appear on the screen</t>
   </si>
   <si>
@@ -790,9 +784,6 @@
     <t>Element not verified</t>
   </si>
   <si>
-    <t xml:space="preserve">DeleteProductfromViewCart succesfully </t>
-  </si>
-  <si>
     <t>action click failed</t>
   </si>
   <si>
@@ -802,137 +793,9 @@
     <t>all</t>
   </si>
   <si>
-    <t>Add product successfully</t>
-  </si>
-  <si>
-    <t>Select Substitute successfully: Do Not Allow Substitute for product: null</t>
-  </si>
-  <si>
-    <t>Select Substitute successfully: Allow Substitute for product: null</t>
-  </si>
-  <si>
-    <t>Select slot Fail: 2Sep for product: 06:00 PM-07:00 PM</t>
-  </si>
-  <si>
-    <t>Text Entered successfully: userchandna5593954@mailinator.com</t>
-  </si>
-  <si>
     <t>City Market Norwalk - Online Grocery Supermarket with Home Delivery</t>
   </si>
   <si>
-    <t>Title verified succesfully: City Market Norwalk - Online Grocery Supermarket with Home Delivery</t>
-  </si>
-  <si>
-    <t>text mismatch: Your card's security code is incomplete</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 29 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\WINDOWS\TEMP\scoped_dir8284_2642}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: c73506e288936c03f1d867791e0dd740
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 58 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\WINDOWS\TEMP\scoped_dir8284_2642}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: c73506e288936c03f1d867791e0dd740
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>element not visible
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 28 milliseconds
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\WINDOWS\TEMP\scoped_dir8284_2642}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: c73506e288936c03f1d867791e0dd740</t>
-  </si>
-  <si>
-    <t>"4 Sep"</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 30 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir8564_16081}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 06c4f7d7d3541e1fcd4d749faf568d0f
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 18 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir8564_16081}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 06c4f7d7d3541e1fcd4d749faf568d0f
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>Select Slot successfully: 4 Sep  06:00 PM-07:00 PM</t>
-  </si>
-  <si>
-    <t>text verified: Your card's security code is incomplete</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move and Add product Fail </t>
-  </si>
-  <si>
-    <t>action Move and add product failed: exist</t>
-  </si>
-  <si>
-    <t>bound must be positive</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 15 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\WINDOWS\TEMP\scoped_dir2304_5586}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 3029accc9e73fa132c825781c7109fc7
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 19 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\WINDOWS\TEMP\scoped_dir2304_5586}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 3029accc9e73fa132c825781c7109fc7
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
     <t>VerifyTitle: City Market Norwalk - Online Grocery Supermarket with Home Delivery</t>
   </si>
   <si>
@@ -999,959 +862,16 @@
     <t>SetText: 1234567890</t>
   </si>
   <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 38 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13564_28830}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 3fddb53966380820a83efadd593af767
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 64 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13564_28830}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 3fddb53966380820a83efadd593af767
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
     <t>SetText: 06820</t>
   </si>
   <si>
     <t>SelectSlot: 4 Sep</t>
   </si>
   <si>
-    <t>element not visible
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 37 milliseconds
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13564_28830}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 3fddb53966380820a83efadd593af767</t>
-  </si>
-  <si>
     <t>VerifyText: Your card's security code is incomplete</t>
   </si>
   <si>
     <t>DeleteProductfromViewCart: all</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 17 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir4916_13851}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 91c945a792718f57b1adc546c6b8d178
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 52 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir4916_13851}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 91c945a792718f57b1adc546c6b8d178
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>element not visible
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 23 milliseconds
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir4916_13851}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 91c945a792718f57b1adc546c6b8d178</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'My Account')]"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 10 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//a[contains(text(),'My Account')]}</t>
-  </si>
-  <si>
-    <t>action set text failed: Randomemailid</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-sociallogin-popup-email"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 18 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=id, value=magestore-sociallogin-popup-email}</t>
-  </si>
-  <si>
-    <t>action set text failed: 123456</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-sociallogin-popup-pass"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 15 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=id, value=magestore-sociallogin-popup-pass}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-button-sociallogin"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 13 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=id, value=magestore-button-sociallogin}</t>
-  </si>
-  <si>
-    <t>text not verified: Akash sangal</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //*[@id="wrap"]/header/div[1]/div/div[2]/ul/li[1]/span/span (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d</t>
-  </si>
-  <si>
-    <t>action MoveToProductList failed: Quick &amp; Easy Food Solutions</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 18 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']}</t>
-  </si>
-  <si>
-    <t>action Move and add product failed: null</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 16 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 11 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>action Move and add product failed: Banquet Brown 'N Serve Turkey Sausage Links</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 10 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 15 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 13 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>action Move and add product failed: College Inn Fat Free &amp; Lower Sodium Chicken Broth - 32oz</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 14 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[normalize-space(@class) = 'action showcart icon icon-main-cart']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 17 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//a[normalize-space(@class) = 'action showcart icon icon-main-cart']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[normalize-space(@class) = 'action viewcart btn btn__hollow btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 19 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//a[normalize-space(@class) = 'action viewcart btn btn__hollow btn-block']}</t>
-  </si>
-  <si>
-    <t>action Select Substitute failed: Do Not Allow Substitute</t>
-  </si>
-  <si>
-    <t>action Select Substitute failed: Allow Substitute</t>
-  </si>
-  <si>
-    <t>action VerifySummaryViewCart failed: null  null</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":".//div[normalize-space(@class) = 'cart-empty']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 11 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=.//div[normalize-space(@class) = 'cart-empty']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'action primary checkout']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 16 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'action primary checkout']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'button action continue primary btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 21 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'button action continue primary btn-block']}</t>
-  </si>
-  <si>
-    <t>text not verified: Please select delivery slot.</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //div[normalize-space(@class) = 'message notice'] (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d</t>
-  </si>
-  <si>
-    <t>action set text failed: ChandnaUserAddress</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Street Address']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 19 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Street Address']}</t>
-  </si>
-  <si>
-    <t>action set text failed: ChandnaUserCity</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'City']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 14 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'City']}</t>
-  </si>
-  <si>
-    <t>action set text failed: 068202322</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Zip/Postal Code']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 14 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Zip/Postal Code']}</t>
-  </si>
-  <si>
-    <t>action set text failed: 1234567890</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Phone Number']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 14 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Phone Number']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 25 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 22 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>action set text failed: 06820</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Zip/Postal Code']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 10 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Zip/Postal Code']}</t>
-  </si>
-  <si>
-    <t>action Select slot failed: 4 Sep  06:00 PM-07:00 PM</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 10 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'button action continue primary btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 13 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'button action continue primary btn-block']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'action primary checkout']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 15 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'action primary checkout']}</t>
-  </si>
-  <si>
-    <t>text not verified: Your card's security code is incomplete</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.id: cryozonic-stripe-card-errors (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[normalize-space(@class) = 'pull-right']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 24 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//a[normalize-space(@class) = 'pull-right']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[contains(text(),'Akash')]"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 21 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//span[contains(text(),'Akash')]}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'Sign Out')]"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 18 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17096_21656}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 0f370b59264a5c9c3e552ca3b87e2a7d
-*** Element info: {Using=xpath, value=//a[contains(text(),'Sign Out')]}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'My Account')]"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 14 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//a[contains(text(),'My Account')]}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-sociallogin-popup-email"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 27 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=id, value=magestore-sociallogin-popup-email}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-sociallogin-popup-pass"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 25 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=id, value=magestore-sociallogin-popup-pass}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"id","selector":"magestore-button-sociallogin"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 26 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=id, value=magestore-button-sociallogin}</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //*[@id="wrap"]/header/div[1]/div/div[2]/ul/li[1]/span/span (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 27 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//ul[normalize-space(@class) = 'nav-primary mmenu__parent-list']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 60 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 23 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 41 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 43 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 39 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 40 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 33 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//div[normalize-space(@class) = 'products wrapper cp__products-wrapper grid products-grid']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[normalize-space(@class) = 'action showcart icon icon-main-cart']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 26 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//a[normalize-space(@class) = 'action showcart icon icon-main-cart']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[normalize-space(@class) = 'action viewcart btn btn__hollow btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 21 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//a[normalize-space(@class) = 'action viewcart btn btn__hollow btn-block']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":".//div[normalize-space(@class) = 'cart-empty']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 41 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=.//div[normalize-space(@class) = 'cart-empty']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'action primary checkout']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 28 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'action primary checkout']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'button action continue primary btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 28 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'button action continue primary btn-block']}</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //div[normalize-space(@class) = 'message notice'] (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Street Address']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 29 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Street Address']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'City']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 41 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'City']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Zip/Postal Code']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 29 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Zip/Postal Code']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Phone Number']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 31 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Phone Number']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 35 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 68 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//input[normalize-space(@placeholder) = 'Zip/Postal Code']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 18 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//input[normalize-space(@placeholder) = 'Zip/Postal Code']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 20 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'button action continue primary btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 29 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'button action continue primary btn-block']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'action primary checkout']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 32 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'action primary checkout']}</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.id: cryozonic-stripe-card-errors (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.29.134', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[normalize-space(@class) = 'pull-right']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 28 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//a[normalize-space(@class) = 'pull-right']}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//span[contains(text(),'Akash')]"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 32 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//span[contains(text(),'Akash')]}</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//a[contains(text(),'Sign Out')]"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 32 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir12644_3729}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 61816d28be1bbd78b3d2429a87a9572e
-*** Element info: {Using=xpath, value=//a[contains(text(),'Sign Out')]}</t>
   </si>
   <si>
     <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
@@ -1989,6 +909,86 @@
 Driver info: org.openqa.selenium.chrome.ChromeDriver
 Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir5748_14413}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
 Session ID: 0a6edcb7a5ce9e8996ef2813ea87b4d0</t>
+  </si>
+  <si>
+    <t>"6 Sep"</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 26 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13124_418}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 1a9eb8faadaec50215f32bb72e5efa1c
+*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 18 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13124_418}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 1a9eb8faadaec50215f32bb72e5efa1c
+*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
+  </si>
+  <si>
+    <t>SelectSlot: 6 Sep</t>
+  </si>
+  <si>
+    <t>element not visible
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 18 milliseconds
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir13124_418}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 1a9eb8faadaec50215f32bb72e5efa1c</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 33 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17476_28541}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 37907ebc46879002404769a61233699b
+*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//table[normalize-space(@class) = 'table time-slot']"}
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 22 milliseconds
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17476_28541}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 37907ebc46879002404769a61233699b
+*** Element info: {Using=xpath, value=//table[normalize-space(@class) = 'table time-slot']}</t>
+  </si>
+  <si>
+    <t>element not visible
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 21 milliseconds
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17476_28541}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 37907ebc46879002404769a61233699b</t>
   </si>
 </sst>
 </file>
@@ -2645,7 +1645,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2653,7 +1653,7 @@
         <v>87</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2666,7 +1666,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>215</v>
@@ -2674,33 +1674,33 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>226</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="A5:D5"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2711,7 +1711,7 @@
   <dimension ref="A1:O59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C50" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="G50" sqref="G50"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultRowHeight="41.25"/>
@@ -2778,7 +1778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row ht="180" r="2" spans="1:15">
+    <row ht="135" r="2" spans="1:15">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -2794,7 +1794,7 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -2803,7 +1803,7 @@
         <v>36</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>107</v>
@@ -2842,7 +1842,7 @@
         <v>40</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>107</v>
@@ -2881,7 +1881,7 @@
         <v>42</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>107</v>
@@ -2920,7 +1920,7 @@
         <v>46</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>107</v>
@@ -2932,7 +1932,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="120" r="6" spans="1:15">
+    <row ht="45" r="6" spans="1:15">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2965,7 +1965,7 @@
         <v>52</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>107</v>
@@ -2977,7 +1977,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="60" r="7" spans="1:15">
+    <row ht="45" r="7" spans="1:15">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
@@ -3006,7 +2006,7 @@
         <v>57</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>277</v>
+        <v>254</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>107</v>
@@ -3045,7 +2045,7 @@
         <v>61</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>107</v>
@@ -3086,7 +2086,7 @@
         <v>66</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>278</v>
+        <v>255</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>107</v>
@@ -3098,7 +2098,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="180" r="10" spans="1:15">
+    <row ht="135" r="10" spans="1:15">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
@@ -3114,7 +2114,7 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3123,7 +2123,7 @@
         <v>36</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>107</v>
@@ -3162,7 +2162,7 @@
         <v>36</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>107</v>
@@ -3205,7 +2205,7 @@
         <v>36</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>107</v>
@@ -3244,7 +2244,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>107</v>
@@ -3276,7 +2276,7 @@
         <v>85</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="4"/>
@@ -3285,7 +2285,7 @@
         <v>36</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>107</v>
@@ -3297,7 +2297,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="75" r="15" spans="1:15">
+    <row ht="120" r="15" spans="1:15">
       <c r="A15" s="4" t="s">
         <v>17</v>
       </c>
@@ -3326,7 +2326,7 @@
         <v>36</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>282</v>
+        <v>259</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>107</v>
@@ -3358,7 +2358,7 @@
         <v>85</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -3367,7 +2367,7 @@
         <v>36</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>107</v>
@@ -3406,10 +2406,10 @@
         <v>36</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>108</v>
@@ -3438,7 +2438,7 @@
         <v>85</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -3447,7 +2447,7 @@
         <v>36</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>107</v>
@@ -3459,7 +2459,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="75" r="19" spans="1:15">
+    <row ht="135" r="19" spans="1:15">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -3488,7 +2488,7 @@
         <v>36</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>107</v>
@@ -3520,7 +2520,7 @@
         <v>85</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -3529,7 +2529,7 @@
         <v>36</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>107</v>
@@ -3541,7 +2541,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="75" r="21" spans="1:15">
+    <row ht="135" r="21" spans="1:15">
       <c r="A21" s="4" t="s">
         <v>17</v>
       </c>
@@ -3570,7 +2570,7 @@
         <v>36</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>283</v>
+        <v>260</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>107</v>
@@ -3602,7 +2602,7 @@
         <v>85</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -3611,7 +2611,7 @@
         <v>36</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>281</v>
+        <v>258</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>107</v>
@@ -3650,7 +2650,7 @@
         <v>36</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>107</v>
@@ -3689,7 +2689,7 @@
         <v>36</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>107</v>
@@ -3728,7 +2728,7 @@
         <v>36</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>107</v>
@@ -3767,7 +2767,7 @@
         <v>98</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M26" s="4" t="s">
         <v>107</v>
@@ -3779,7 +2779,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="135" r="27" spans="1:15">
+    <row ht="60" r="27" spans="1:15">
       <c r="A27" s="4" t="s">
         <v>17</v>
       </c>
@@ -3808,7 +2808,7 @@
         <v>104</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>107</v>
@@ -3820,7 +2820,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="120" r="28" spans="1:15">
+    <row ht="60" r="28" spans="1:15">
       <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
@@ -3849,7 +2849,7 @@
         <v>104</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>107</v>
@@ -3861,7 +2861,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="120" r="29" spans="1:15">
+    <row ht="60" r="29" spans="1:15">
       <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
@@ -3890,7 +2890,7 @@
         <v>104</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>107</v>
@@ -3902,7 +2902,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="135" r="30" spans="1:15">
+    <row ht="60" r="30" spans="1:15">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
@@ -3931,7 +2931,7 @@
         <v>104</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>284</v>
+        <v>261</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>107</v>
@@ -3943,7 +2943,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="120" r="31" spans="1:15">
+    <row ht="60" r="31" spans="1:15">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
@@ -3972,7 +2972,7 @@
         <v>104</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>107</v>
@@ -3984,7 +2984,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="120" r="32" spans="1:15">
+    <row ht="60" r="32" spans="1:15">
       <c r="A32" s="4" t="s">
         <v>17</v>
       </c>
@@ -4013,7 +3013,7 @@
         <v>104</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>285</v>
+        <v>262</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>107</v>
@@ -4025,7 +3025,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="60" r="33" spans="1:15">
+    <row ht="45" r="33" spans="1:15">
       <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
@@ -4052,7 +3052,7 @@
         <v>121</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>286</v>
+        <v>263</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>107</v>
@@ -4064,7 +3064,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="60" r="34" spans="1:15">
+    <row ht="15" r="34" spans="1:15">
       <c r="A34" s="4" t="s">
         <v>17</v>
       </c>
@@ -4089,7 +3089,7 @@
         <v>201</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>287</v>
+        <v>264</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>107</v>
@@ -4128,7 +3128,7 @@
         <v>151</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>107</v>
@@ -4165,7 +3165,7 @@
         <v>154</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>288</v>
+        <v>265</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>107</v>
@@ -4202,7 +3202,7 @@
         <v>201</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>107</v>
@@ -4241,7 +3241,7 @@
         <v>157</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M38" s="4" t="s">
         <v>107</v>
@@ -4282,7 +3282,7 @@
         <v>161</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>290</v>
+        <v>267</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>107</v>
@@ -4323,7 +3323,7 @@
         <v>165</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>107</v>
@@ -4364,7 +3364,7 @@
         <v>166</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>107</v>
@@ -4396,7 +3396,7 @@
         <v>185</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -4405,7 +3405,7 @@
         <v>171</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>293</v>
+        <v>270</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>107</v>
@@ -4446,7 +3446,7 @@
         <v>172</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>294</v>
+        <v>271</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>107</v>
@@ -4493,7 +3493,7 @@
         <v>206</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>388</v>
+        <v>284</v>
       </c>
       <c r="O44" s="4" t="s">
         <v>152</v>
@@ -4524,7 +3524,7 @@
         <v>201</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>107</v>
@@ -4544,10 +3544,10 @@
         <v>58</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>29</v>
@@ -4560,16 +3560,16 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>206</v>
       </c>
       <c r="N46" s="4" t="s">
-        <v>389</v>
+        <v>285</v>
       </c>
       <c r="O46" s="4" t="s">
         <v>152</v>
@@ -4604,7 +3604,7 @@
         <v>171</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>297</v>
+        <v>272</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>107</v>
@@ -4641,7 +3641,7 @@
         <v>201</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="M48" s="4" t="s">
         <v>107</v>
@@ -4661,7 +3661,7 @@
         <v>32</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>38</v>
@@ -4680,7 +3680,7 @@
         <v>180</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>107</v>
@@ -4712,7 +3712,7 @@
         <v>178</v>
       </c>
       <c r="G50" s="12" t="s">
-        <v>263</v>
+        <v>279</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>179</v>
@@ -4723,7 +3723,7 @@
         <v>180</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>206</v>
@@ -4737,7 +3737,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="51" spans="1:15">
       <c r="A51" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>27</v>
@@ -4762,7 +3762,7 @@
         <v>204</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M51" s="4" t="s">
         <v>107</v>
@@ -4776,13 +3776,13 @@
     </row>
     <row customHeight="1" ht="41.25" r="52" spans="1:15">
       <c r="A52" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>28</v>
@@ -4798,16 +3798,16 @@
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M52" s="4" t="s">
         <v>206</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>390</v>
+        <v>286</v>
       </c>
       <c r="O52" s="4" t="s">
         <v>152</v>
@@ -4815,13 +3815,13 @@
     </row>
     <row customHeight="1" ht="41.25" r="53" spans="1:15">
       <c r="A53" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>64</v>
@@ -4830,10 +3830,10 @@
         <v>50</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -4842,7 +3842,7 @@
         <v>161</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="M53" s="4" t="s">
         <v>206</v>
@@ -4856,13 +3856,13 @@
     </row>
     <row customHeight="1" ht="41.25" r="54" spans="1:15">
       <c r="A54" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>28</v>
@@ -4871,17 +3871,17 @@
         <v>29</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>107</v>
@@ -4895,16 +3895,16 @@
     </row>
     <row customHeight="1" ht="41.25" r="55" spans="1:15">
       <c r="A55" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E55" s="4" t="s">
         <v>29</v>
@@ -4913,16 +3913,16 @@
         <v>102</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="M55" s="4" t="s">
         <v>107</v>
@@ -4936,13 +3936,13 @@
     </row>
     <row customHeight="1" ht="41.25" r="56" spans="1:15">
       <c r="A56" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>28</v>
@@ -4951,17 +3951,17 @@
         <v>29</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>107</v>
@@ -4975,13 +3975,13 @@
     </row>
     <row customHeight="1" ht="41.25" r="57" spans="1:15">
       <c r="A57" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>28</v>
@@ -4990,7 +3990,7 @@
         <v>29</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
@@ -5000,7 +4000,7 @@
         <v>204</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>275</v>
+        <v>252</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>107</v>
@@ -5014,13 +4014,13 @@
     </row>
     <row customHeight="1" ht="41.25" r="58" spans="1:15">
       <c r="A58" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>199</v>
@@ -5035,7 +4035,7 @@
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
       <c r="L58" s="4" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="M58" s="4" t="s">
         <v>107</v>
@@ -5049,7 +4049,7 @@
     </row>
     <row customHeight="1" ht="41.25" r="59" spans="1:15">
       <c r="A59" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>53</v>
@@ -5064,7 +4064,7 @@
         <v>29</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
@@ -5074,7 +4074,7 @@
         <v>40</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>274</v>
+        <v>251</v>
       </c>
       <c r="M59" s="4" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
changes in checkout slot execution
changes in checkout slot execution
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.Checkout.xlsx
+++ b/lib_testcase/com.aislend.Checkout.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="281">
   <si>
     <t>Action</t>
   </si>
@@ -793,9 +793,6 @@
     <t>Click: null</t>
   </si>
   <si>
-    <t>SetText: Randomemailid</t>
-  </si>
-  <si>
     <t>SetText: 123456</t>
   </si>
   <si>
@@ -835,9 +832,6 @@
     <t>Wait: 6000</t>
   </si>
   <si>
-    <t>VerifyText: Please select delivery slot.</t>
-  </si>
-  <si>
     <t>SetText: ChandnaUserAddress</t>
   </si>
   <si>
@@ -853,56 +847,16 @@
     <t>SetText: 06820</t>
   </si>
   <si>
-    <t>VerifyText: Your card's security code is incomplete</t>
-  </si>
-  <si>
     <t>DeleteProductfromViewCart: all</t>
   </si>
   <si>
     <t>"11 Sep"</t>
   </si>
   <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 19 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir11216_31392}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: b746c4669419dfc4e89e18d636541a91
-*** Element info: {Using=xpath, value=//textarea[normalize-space(@placeholder) = 'Order Instructions']}</t>
-  </si>
-  <si>
     <t>SelectSlot: 11 Sep</t>
   </si>
   <si>
     <t>action click failed</t>
-  </si>
-  <si>
-    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[normalize-space(@class) = 'button action continue primary btn-block']"}
-  (Session info: chrome=68.0.3440.106)
-  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
-Command duration or timeout: 17 milliseconds
-For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir11912_29672}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 1a35c3999676c4eb04cb6f7f8a978a85
-*** Element info: {Using=xpath, value=//button[normalize-space(@class) = 'button action continue primary btn-block']}</t>
-  </si>
-  <si>
-    <t>text not verified: Please select delivery slot.</t>
-  </si>
-  <si>
-    <t>Expected condition failed: waiting for presence of element located by: By.xpath: //div[normalize-space(@class) = 'message notice'] (tried for 40 second(s) with 500 MILLISECONDS interval)
-Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
-System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
-Driver info: org.openqa.selenium.chrome.ChromeDriver
-Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir11912_29672}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
-Session ID: 1a35c3999676c4eb04cb6f7f8a978a85</t>
   </si>
   <si>
     <t>no such element: Unable to locate element: {"method":"xpath","selector":"//textarea[normalize-space(@placeholder) = 'Order Instructions']"}
@@ -940,6 +894,24 @@
 Driver info: org.openqa.selenium.chrome.ChromeDriver
 Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir11912_29672}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
 Session ID: 1a35c3999676c4eb04cb6f7f8a978a85</t>
+  </si>
+  <si>
+    <t>userchandna7049580@mailinator.com</t>
+  </si>
+  <si>
+    <t>SetText: userchandna7049580@mailinator.com</t>
+  </si>
+  <si>
+    <t>VerifyText: Please select delivery slot.</t>
+  </si>
+  <si>
+    <t>//textarea[normalize-space(@placeholder) = 'Delivery Instructions']</t>
+  </si>
+  <si>
+    <t>SetText: user chandna</t>
+  </si>
+  <si>
+    <t>VerifyText: Your card's security code is incomplete</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0" zoomScale="70" zoomScaleNormal="70">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultRowHeight="41.25"/>
@@ -1883,7 +1855,7 @@
         <v>152</v>
       </c>
     </row>
-    <row ht="45" r="6" spans="1:15">
+    <row ht="75" r="6" spans="1:15">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -1903,7 +1875,7 @@
         <v>51</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>105</v>
+        <v>275</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>105</v>
@@ -1916,7 +1888,7 @@
         <v>52</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>107</v>
@@ -1957,7 +1929,7 @@
         <v>57</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>107</v>
@@ -2037,7 +2009,7 @@
         <v>66</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>107</v>
@@ -2156,7 +2128,7 @@
         <v>36</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>107</v>
@@ -2195,7 +2167,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>107</v>
@@ -2236,7 +2208,7 @@
         <v>36</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>107</v>
@@ -2277,7 +2249,7 @@
         <v>36</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M15" s="4" t="s">
         <v>107</v>
@@ -2318,7 +2290,7 @@
         <v>36</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>107</v>
@@ -2357,10 +2329,10 @@
         <v>36</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N17" s="4" t="s">
         <v>108</v>
@@ -2398,7 +2370,7 @@
         <v>36</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>107</v>
@@ -2439,7 +2411,7 @@
         <v>36</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>107</v>
@@ -2480,7 +2452,7 @@
         <v>36</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>107</v>
@@ -2521,7 +2493,7 @@
         <v>36</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>107</v>
@@ -2562,7 +2534,7 @@
         <v>36</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>107</v>
@@ -2601,7 +2573,7 @@
         <v>36</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>107</v>
@@ -2759,7 +2731,7 @@
         <v>104</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M27" s="4" t="s">
         <v>107</v>
@@ -2800,7 +2772,7 @@
         <v>104</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M28" s="4" t="s">
         <v>107</v>
@@ -2841,7 +2813,7 @@
         <v>104</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M29" s="4" t="s">
         <v>107</v>
@@ -2882,7 +2854,7 @@
         <v>104</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="M30" s="4" t="s">
         <v>107</v>
@@ -2923,7 +2895,7 @@
         <v>104</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M31" s="4" t="s">
         <v>107</v>
@@ -2964,7 +2936,7 @@
         <v>104</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M32" s="4" t="s">
         <v>107</v>
@@ -3003,7 +2975,7 @@
         <v>121</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="M33" s="4" t="s">
         <v>107</v>
@@ -3040,7 +3012,7 @@
         <v>201</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>107</v>
@@ -3116,7 +3088,7 @@
         <v>154</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M36" s="4" t="s">
         <v>107</v>
@@ -3153,7 +3125,7 @@
         <v>201</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M37" s="4" t="s">
         <v>107</v>
@@ -3192,13 +3164,13 @@
         <v>157</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>275</v>
+        <v>108</v>
       </c>
       <c r="O38" s="4" t="s">
         <v>152</v>
@@ -3233,13 +3205,13 @@
         <v>161</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>277</v>
+        <v>108</v>
       </c>
       <c r="O39" s="4" t="s">
         <v>152</v>
@@ -3274,7 +3246,7 @@
         <v>165</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="M40" s="4" t="s">
         <v>107</v>
@@ -3315,7 +3287,7 @@
         <v>166</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>107</v>
@@ -3356,7 +3328,7 @@
         <v>171</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M42" s="4" t="s">
         <v>107</v>
@@ -3397,7 +3369,7 @@
         <v>172</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M43" s="4" t="s">
         <v>107</v>
@@ -3426,7 +3398,7 @@
         <v>29</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>187</v>
+        <v>278</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>174</v>
@@ -3438,13 +3410,13 @@
         <v>175</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>210</v>
+        <v>279</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N44" s="4" t="s">
-        <v>278</v>
+        <v>108</v>
       </c>
       <c r="O44" s="4" t="s">
         <v>152</v>
@@ -3475,7 +3447,7 @@
         <v>201</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M45" s="4" t="s">
         <v>107</v>
@@ -3516,7 +3488,7 @@
         <v>171</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M46" s="4" t="s">
         <v>107</v>
@@ -3553,7 +3525,7 @@
         <v>201</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M47" s="4" t="s">
         <v>107</v>
@@ -3624,7 +3596,7 @@
         <v>178</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>179</v>
@@ -3635,7 +3607,7 @@
         <v>180</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>107</v>
@@ -3713,13 +3685,13 @@
         <v>231</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>274</v>
+        <v>248</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>279</v>
+        <v>108</v>
       </c>
       <c r="O51" s="4" t="s">
         <v>152</v>
@@ -3757,10 +3729,10 @@
         <v>280</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N52" s="4" t="s">
-        <v>281</v>
+        <v>108</v>
       </c>
       <c r="O52" s="4" t="s">
         <v>152</v>
@@ -3834,7 +3806,7 @@
         <v>235</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>107</v>
@@ -3947,7 +3919,7 @@
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
       <c r="L57" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="M57" s="4" t="s">
         <v>107</v>

</xml_diff>

<commit_message>
updated logger and refactoring for stable execution
updated logger and refactoring for stable execution
</commit_message>
<xml_diff>
--- a/lib_testcase/com.aislend.Checkout.xlsx
+++ b/lib_testcase/com.aislend.Checkout.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1728" uniqueCount="280">
   <si>
     <t>Action</t>
   </si>
@@ -878,6 +878,20 @@
   </si>
   <si>
     <t>bound must be positive</t>
+  </si>
+  <si>
+    <t>action click failed</t>
+  </si>
+  <si>
+    <t>element not visible
+  (Session info: chrome=68.0.3440.106)
+  (Driver info: chromedriver=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91),platform=Windows NT 10.0.17134 x86_64) (WARNING: The server did not provide any stacktrace information)
+Command duration or timeout: 25 milliseconds
+Build info: version: 'unknown', revision: '1969d75', time: '2016-10-18 09:43:45 -0700'
+System info: host: 'DESKTOP-OEL817D', ip: '192.168.134.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '1.8.0_161'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities [{applicationCacheEnabled=false, rotatable=false, mobileEmulationEnabled=false, networkConnectionEnabled=false, chrome={chromedriverVersion=2.36.540470 (e522d04694c7ebea4ba8821272dbef4f9b818c91), userDataDir=C:\Users\Akash\AppData\Local\Temp\scoped_dir17800_878}, takesHeapSnapshot=true, pageLoadStrategy=normal, databaseEnabled=false, handlesAlerts=true, hasTouchScreen=false, version=68.0.3440.106, platform=XP, browserConnectionEnabled=false, nativeEvents=true, acceptSslCerts=false, acceptInsecureCerts=false, locationContextEnabled=true, webStorageEnabled=true, browserName=chrome, takesScreenshot=true, javascriptEnabled=true, cssSelectorsEnabled=true, setWindowRect=true, unexpectedAlertBehaviour=}]
+Session ID: 90c707c1cf12f41c381b5a6a3677976b</t>
   </si>
 </sst>
 </file>
@@ -2174,13 +2188,13 @@
         <v>36</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>276</v>
+        <v>253</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>206</v>
+        <v>107</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>277</v>
+        <v>108</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>152</v>
@@ -3576,7 +3590,7 @@
         <v>269</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="N49" s="4" t="s">
         <v>108</v>
@@ -3651,13 +3665,13 @@
         <v>231</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>248</v>
+        <v>278</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>108</v>
+        <v>279</v>
       </c>
       <c r="O51" s="4" t="s">
         <v>152</v>
@@ -3695,7 +3709,7 @@
         <v>274</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>108</v>

</xml_diff>